<commit_message>
Updating the plot for the paper
</commit_message>
<xml_diff>
--- a/Shiny Apps/DTEAssurance/ControlSample.xlsx
+++ b/Shiny Apps/DTEAssurance/ControlSample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smp21js\Documents\PhD-Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smp21js\Documents\R Projects\PhD-Materials\Shiny Apps\DTEAssurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F647BB06-5D01-4F1D-8917-A452C074CFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE65FE0-5854-466F-A12E-A86CF5958BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>time</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>cens</t>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>